<commit_message>
Assging scenario based analysis
</commit_message>
<xml_diff>
--- a/6_Advanced_Data_Analysis/1_Analysis_Add-ins_DIVALK.xlsx
+++ b/6_Advanced_Data_Analysis/1_Analysis_Add-ins_DIVALK.xlsx
@@ -8,56 +8,63 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\StudyMaterials\Excel\Excel_Data_Analytics_Course-main\Excel_Data_Analytics_Course-main\6_Advanced_Data_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23283256-C5C1-4667-BF96-BB71D45B24D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46974101-E01B-4138-9587-72E04C8E7B09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{6C37AC85-509F-4D10-9DB1-F70D16D6FBAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="8" xr2:uid="{6C37AC85-509F-4D10-9DB1-F70D16D6FBAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="16" r:id="rId1"/>
     <sheet name="Forecast_Original" sheetId="7" r:id="rId2"/>
     <sheet name="Forecast_Final" sheetId="8" state="hidden" r:id="rId3"/>
     <sheet name="Scenario Summary" sheetId="23" r:id="rId4"/>
-    <sheet name="What-If_Analysis" sheetId="3" r:id="rId5"/>
-    <sheet name="Scenario_Summary" sheetId="12" state="hidden" r:id="rId6"/>
-    <sheet name="Answer_Report" sheetId="13" state="hidden" r:id="rId7"/>
-    <sheet name="Limits_Report" sheetId="15" state="hidden" r:id="rId8"/>
+    <sheet name="Answer Report 1" sheetId="30" r:id="rId5"/>
+    <sheet name="Sensitivity Report 1" sheetId="31" r:id="rId6"/>
+    <sheet name="Limits Report 1" sheetId="32" r:id="rId7"/>
+    <sheet name="Answer Report 2" sheetId="33" r:id="rId8"/>
+    <sheet name="What-If_Analysis" sheetId="3" r:id="rId9"/>
+    <sheet name="Scenario_Summary" sheetId="12" state="hidden" r:id="rId10"/>
+    <sheet name="Answer_Report" sheetId="13" state="hidden" r:id="rId11"/>
+    <sheet name="Limits_Report" sheetId="15" state="hidden" r:id="rId12"/>
   </sheets>
   <definedNames>
-    <definedName name="base" localSheetId="4">'What-If_Analysis'!$C$3</definedName>
-    <definedName name="bonus" localSheetId="4">'What-If_Analysis'!$C$4</definedName>
-    <definedName name="raise" localSheetId="4">'What-If_Analysis'!$C$5</definedName>
-    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'What-If_Analysis'!$C$4</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'What-If_Analysis'!$C$5</definedName>
-    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rhs1" localSheetId="4" hidden="1">0.25</definedName>
-    <definedName name="solver_rhs2" localSheetId="4" hidden="1">0.035</definedName>
-    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="7" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="base" localSheetId="8">'What-If_Analysis'!$C$3</definedName>
+    <definedName name="bonus" localSheetId="8">'What-If_Analysis'!$C$4</definedName>
+    <definedName name="raise" localSheetId="8">'What-If_Analysis'!$C$5</definedName>
+    <definedName name="solver_adj" localSheetId="8" hidden="1">'What-If_Analysis'!$C$4:$C$5</definedName>
+    <definedName name="solver_cvg" localSheetId="8" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="8" hidden="1">'What-If_Analysis'!$C$4</definedName>
+    <definedName name="solver_lhs2" localSheetId="8" hidden="1">'What-If_Analysis'!$C$5</definedName>
+    <definedName name="solver_mip" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="8" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="8" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_nwt" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="8" hidden="1">'What-If_Analysis'!$C$14</definedName>
+    <definedName name="solver_pre" localSheetId="8" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="8" hidden="1">0.2</definedName>
+    <definedName name="solver_rhs2" localSheetId="8" hidden="1">0.05</definedName>
+    <definedName name="solver_rlx" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="8" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="8" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="6" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="11" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="8" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="8" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="8" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="8" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="8" hidden="1">3</definedName>
+    <definedName name="solver_val" localSheetId="8" hidden="1">640000</definedName>
+    <definedName name="solver_ver" localSheetId="8" hidden="1">3</definedName>
     <definedName name="TotalSalary">'What-If_Analysis'!$C$14</definedName>
     <definedName name="Year0">'What-If_Analysis'!$C$9</definedName>
     <definedName name="Year1">'What-If_Analysis'!$C$10</definedName>
@@ -86,7 +93,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="94">
   <si>
     <t>Base Salary</t>
   </si>
@@ -329,12 +336,55 @@
   <si>
     <t>Created by Dell on 6/19/2025</t>
   </si>
+  <si>
+    <t>Worksheet: [1_Analysis_Add-ins_DIVALK.xlsx]What-If_Analysis</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.032 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 2 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Gradient</t>
+  </si>
+  <si>
+    <t>Lagrange</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>Report Created: 6/19/2025 7:35:27 PM</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.047 Seconds.</t>
+  </si>
+  <si>
+    <t>Report Created: 6/19/2025 8:35:29 PM</t>
+  </si>
+  <si>
+    <t>$C$4&lt;=0.2</t>
+  </si>
+  <si>
+    <t>$C$5&lt;=0.05</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
@@ -887,7 +937,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -1021,21 +1071,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -14995,7 +15046,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FFF88A0-A9A7-4704-93B2-AFBC3DCAB515}">
   <dimension ref="A1:E427"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D368" sqref="D368"/>
     </sheetView>
   </sheetViews>
@@ -18506,7 +18557,7 @@
         <v>66.716957191670204</v>
       </c>
       <c r="D399" s="17">
-        <f t="shared" ref="D399:D430" si="4">C399-_xlfn.FORECAST.ETS.CONFINT(A399,$B$2:$B$366,$A$2:$A$366,0.95,1,1)</f>
+        <f t="shared" ref="D399:D427" si="4">C399-_xlfn.FORECAST.ETS.CONFINT(A399,$B$2:$B$366,$A$2:$A$366,0.95,1,1)</f>
         <v>-27.387538454538941</v>
       </c>
       <c r="E399" s="17">
@@ -18996,6 +19047,688 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A599BE6-2460-4FFE-AEBD-9B11D5253C2E}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="B1:G18"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="11.5546875" bestFit="1" customWidth="1" outlineLevel="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="22"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="2:7" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="64.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="E4" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+    </row>
+    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="18">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="29">
+        <v>100000</v>
+      </c>
+      <c r="F6" s="29">
+        <v>80000</v>
+      </c>
+      <c r="G6" s="29">
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="19">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="30">
+        <v>0.1</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0.15</v>
+      </c>
+      <c r="G7" s="30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="20">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E8" s="31">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F8" s="31">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G8" s="31">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="18">
+        <v>110000</v>
+      </c>
+      <c r="E10" s="18">
+        <v>110000</v>
+      </c>
+      <c r="F10" s="18">
+        <v>92000</v>
+      </c>
+      <c r="G10" s="18">
+        <v>126000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="18">
+        <v>111650</v>
+      </c>
+      <c r="E11" s="18">
+        <v>111650</v>
+      </c>
+      <c r="F11" s="18">
+        <v>93104</v>
+      </c>
+      <c r="G11" s="18">
+        <v>127008</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="18">
+        <v>113324.75</v>
+      </c>
+      <c r="E12" s="18">
+        <v>113324.75</v>
+      </c>
+      <c r="F12" s="18">
+        <v>94221.248000000007</v>
+      </c>
+      <c r="G12" s="18">
+        <v>128024.064</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="18">
+        <v>115024.62125</v>
+      </c>
+      <c r="E13" s="18">
+        <v>115024.62125</v>
+      </c>
+      <c r="F13" s="18">
+        <v>95351.902975999998</v>
+      </c>
+      <c r="G13" s="18">
+        <v>129048.25651200001</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="18">
+        <v>116749.99056875</v>
+      </c>
+      <c r="E14" s="18">
+        <v>116749.99056875</v>
+      </c>
+      <c r="F14" s="18">
+        <v>96496.125811712001</v>
+      </c>
+      <c r="G14" s="18">
+        <v>130080.64256409599</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="33">
+        <v>566749.36181875004</v>
+      </c>
+      <c r="E15" s="33">
+        <v>566749.36181875004</v>
+      </c>
+      <c r="F15" s="33">
+        <v>471173.27678771201</v>
+      </c>
+      <c r="G15" s="33">
+        <v>640160.96307609603</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16C6870-2130-42B8-85C2-144B24EA12A8}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="51">
+        <v>640000.63710000005</v>
+      </c>
+      <c r="E16" s="51">
+        <v>640000.63710000005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="52">
+        <v>0.20547045696368638</v>
+      </c>
+      <c r="E21" s="52">
+        <v>0.20547045696368638</v>
+      </c>
+      <c r="F21" s="50" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="53">
+        <v>0.03</v>
+      </c>
+      <c r="E22" s="53">
+        <v>0.03</v>
+      </c>
+      <c r="F22" s="48" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="54">
+        <v>640000.64</v>
+      </c>
+      <c r="E27" s="50" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="50" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="52">
+        <v>0.20547045696368638</v>
+      </c>
+      <c r="E28" s="50" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="50">
+        <v>4.4529543036313624E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="53">
+        <v>0.03</v>
+      </c>
+      <c r="E29" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="48">
+        <v>5.0000000000000044E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B251B97-0E72-44DD-A752-20F45B6DB03B}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.109375" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.109375" customWidth="1"/>
+    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.109375" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="55"/>
+      <c r="C6" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="55"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="51">
+        <v>640000.63710000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="55"/>
+      <c r="C11" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="55"/>
+      <c r="F11" s="55" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="56" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="56" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="52">
+        <v>0.20547045696368638</v>
+      </c>
+      <c r="F13" s="52">
+        <v>0</v>
+      </c>
+      <c r="G13" s="52">
+        <v>530913.57999999996</v>
+      </c>
+      <c r="I13" s="52">
+        <v>0.25</v>
+      </c>
+      <c r="J13" s="52">
+        <v>663641.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="48" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="53">
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="53">
+        <v>0</v>
+      </c>
+      <c r="G14" s="53">
+        <v>602735.23</v>
+      </c>
+      <c r="I14" s="53">
+        <v>0.04</v>
+      </c>
+      <c r="J14" s="53">
+        <v>646429.42000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -26486,7 +27219,9 @@
   </sheetPr>
   <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -26522,16 +27257,15 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="43.2" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="73"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="77" t="s">
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
+      <c r="E4" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="77" t="s">
+      <c r="F4" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="77" t="s">
+      <c r="G4" s="32" t="s">
         <v>79</v>
       </c>
     </row>
@@ -26540,62 +27274,62 @@
         <v>23</v>
       </c>
       <c r="C5" s="25"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
     </row>
     <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="73"/>
-      <c r="C6" s="73" t="s">
+      <c r="B6" s="24"/>
+      <c r="C6" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="68">
+      <c r="D6" s="18">
         <v>80000</v>
       </c>
-      <c r="E6" s="74">
+      <c r="E6" s="29">
         <v>100000</v>
       </c>
-      <c r="F6" s="74">
+      <c r="F6" s="29">
         <v>80000</v>
       </c>
-      <c r="G6" s="74">
+      <c r="G6" s="29">
         <v>120000</v>
       </c>
     </row>
     <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="73"/>
-      <c r="C7" s="73" t="s">
+      <c r="B7" s="24"/>
+      <c r="C7" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="69">
+      <c r="D7" s="19">
         <v>0.1</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="30">
         <v>0.1</v>
       </c>
-      <c r="F7" s="75">
+      <c r="F7" s="30">
         <v>0.15</v>
       </c>
-      <c r="G7" s="75">
+      <c r="G7" s="30">
         <v>0.05</v>
       </c>
     </row>
     <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="73"/>
-      <c r="C8" s="73" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="70">
+      <c r="D8" s="20">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="31">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="F8" s="76">
+      <c r="F8" s="31">
         <v>1.2E-2</v>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="31">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -26604,98 +27338,98 @@
         <v>25</v>
       </c>
       <c r="C9" s="25"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="72"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="72"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
     </row>
     <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="73"/>
-      <c r="C10" s="73" t="s">
+      <c r="B10" s="24"/>
+      <c r="C10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="18">
         <v>88000</v>
       </c>
-      <c r="E10" s="68">
+      <c r="E10" s="18">
         <v>110000</v>
       </c>
-      <c r="F10" s="68">
+      <c r="F10" s="18">
         <v>92000</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="18">
         <v>126000</v>
       </c>
     </row>
     <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="73"/>
-      <c r="C11" s="73" t="s">
+      <c r="B11" s="24"/>
+      <c r="C11" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="68">
+      <c r="D11" s="18">
         <v>89320</v>
       </c>
-      <c r="E11" s="68">
+      <c r="E11" s="18">
         <v>111650</v>
       </c>
-      <c r="F11" s="68">
+      <c r="F11" s="18">
         <v>93104</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="18">
         <v>127008</v>
       </c>
     </row>
     <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="73"/>
-      <c r="C12" s="73" t="s">
+      <c r="B12" s="24"/>
+      <c r="C12" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="68">
+      <c r="D12" s="18">
         <v>90659.8</v>
       </c>
-      <c r="E12" s="68">
+      <c r="E12" s="18">
         <v>113324.75</v>
       </c>
-      <c r="F12" s="68">
+      <c r="F12" s="18">
         <v>94221.248000000007</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="18">
         <v>128024.064</v>
       </c>
     </row>
     <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="73"/>
-      <c r="C13" s="73" t="s">
+      <c r="B13" s="24"/>
+      <c r="C13" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="68">
+      <c r="D13" s="18">
         <v>92019.697</v>
       </c>
-      <c r="E13" s="68">
+      <c r="E13" s="18">
         <v>115024.62125</v>
       </c>
-      <c r="F13" s="68">
+      <c r="F13" s="18">
         <v>95351.902975999998</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="18">
         <v>129048.25651200001</v>
       </c>
     </row>
     <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="73"/>
-      <c r="C14" s="73" t="s">
+      <c r="B14" s="24"/>
+      <c r="C14" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="18">
         <v>93399.992455</v>
       </c>
-      <c r="E14" s="68">
+      <c r="E14" s="18">
         <v>116749.99056875</v>
       </c>
-      <c r="F14" s="68">
+      <c r="F14" s="18">
         <v>96496.125811712001</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="18">
         <v>130080.64256409599</v>
       </c>
     </row>
@@ -26704,16 +27438,16 @@
       <c r="C15" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="71">
+      <c r="D15" s="33">
         <v>453399.48945499997</v>
       </c>
-      <c r="E15" s="71">
+      <c r="E15" s="33">
         <v>566749.36181875004</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="33">
         <v>471173.27678771201</v>
       </c>
-      <c r="G15" s="71">
+      <c r="G15" s="33">
         <v>640160.96307609603</v>
       </c>
     </row>
@@ -26738,11 +27472,785 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{438D79D5-A957-4327-9601-14B3C1F038BA}">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="70">
+        <v>566749.36179999996</v>
+      </c>
+      <c r="E16" s="70">
+        <v>639999.95109999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="71">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="71">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="72">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="E22" s="72">
+        <v>2.1270607913771021E-2</v>
+      </c>
+      <c r="F22" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="70">
+        <v>639999.94999999995</v>
+      </c>
+      <c r="E27" s="67" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="67">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC21EE80-7A79-43B5-BEBD-5445590224A4}">
+  <dimension ref="A1:E15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="73"/>
+      <c r="C7" s="73"/>
+      <c r="D7" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="73" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="69">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="E9" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="67">
+        <v>2.1270607913771E-2</v>
+      </c>
+      <c r="E10" s="67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="73" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="75">
+        <v>639999.94999999995</v>
+      </c>
+      <c r="E15" s="67">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F39C805-ACBC-4E75-A87E-7782867CD4DB}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B6" s="73"/>
+      <c r="C6" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="73"/>
+    </row>
+    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="74" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="70">
+        <v>639999.95109999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B11" s="73"/>
+      <c r="C11" s="73" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="73"/>
+      <c r="F11" s="73" t="s">
+        <v>73</v>
+      </c>
+      <c r="G11" s="73" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="73" t="s">
+        <v>76</v>
+      </c>
+      <c r="J11" s="73" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="I12" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B13" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="71">
+        <v>0.226693026881682</v>
+      </c>
+      <c r="F13" s="71">
+        <v>0</v>
+      </c>
+      <c r="G13" s="71">
+        <v>521727.88</v>
+      </c>
+      <c r="I13" s="69" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="J13" s="69" t="e">
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="72">
+        <v>2.1270607913771021E-2</v>
+      </c>
+      <c r="F14" s="72">
+        <v>0</v>
+      </c>
+      <c r="G14" s="72">
+        <v>613346.51</v>
+      </c>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4E73E3-434A-4FFC-A5E8-13C8314CA87C}">
+  <dimension ref="A1:G29"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="68" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="70">
+        <v>622877.09439999994</v>
+      </c>
+      <c r="E16" s="70">
+        <v>640000.14520000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="68" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="68" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B21" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="71">
+        <v>0.15</v>
+      </c>
+      <c r="E21" s="71">
+        <v>0.17283479610661426</v>
+      </c>
+      <c r="F21" s="69" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="72">
+        <v>0.04</v>
+      </c>
+      <c r="E22" s="72">
+        <v>4.3731865887940702E-2</v>
+      </c>
+      <c r="F22" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="68" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="68" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="G26" s="68" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B27" s="69" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="76">
+        <v>640000.15</v>
+      </c>
+      <c r="E27" s="69" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="G27" s="69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="71">
+        <v>0.17283479610661426</v>
+      </c>
+      <c r="E28" s="69" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="69">
+        <v>2.7165203893385753E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="67" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="72">
+        <v>4.3731865887940702E-2</v>
+      </c>
+      <c r="E29" s="67" t="s">
+        <v>93</v>
+      </c>
+      <c r="F29" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="G29" s="67">
+        <v>6.2681341120593009E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CAB43CA-5103-49AE-8216-4AB866E06AE4}">
   <dimension ref="B1:H14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26778,7 +28286,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="45">
-        <v>80000</v>
+        <v>100000</v>
       </c>
       <c r="E3" s="43" t="s">
         <v>17</v>
@@ -26798,7 +28306,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="46">
-        <v>0.1</v>
+        <v>0.17283479610661426</v>
       </c>
       <c r="E4" s="43" t="s">
         <v>19</v>
@@ -26818,7 +28326,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="47">
-        <v>1.4999999999999999E-2</v>
+        <v>4.3731865887940702E-2</v>
       </c>
       <c r="E5" s="57" t="s">
         <v>21</v>
@@ -26868,7 +28376,7 @@
       </c>
       <c r="C9" s="2">
         <f>(base*(1+raise)^B9)*(1+bonus)</f>
-        <v>88000</v>
+        <v>117283.47961066144</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
@@ -26877,7 +28385,7 @@
       </c>
       <c r="C10" s="2">
         <f>(base*(1+raise)^B10)*(1+bonus)</f>
-        <v>89319.999999999985</v>
+        <v>122412.5050118659</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
@@ -26886,7 +28394,7 @@
       </c>
       <c r="C11" s="2">
         <f>(base*(1+raise)^B11)*(1+bonus)</f>
-        <v>90659.799999999974</v>
+        <v>127765.83226405167</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
@@ -26895,7 +28403,7 @@
       </c>
       <c r="C12" s="2">
         <f>(base*(1+raise)^B12)*(1+bonus)</f>
-        <v>92019.696999999986</v>
+        <v>133353.27050568431</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -26904,7 +28412,7 @@
       </c>
       <c r="C13" s="37">
         <f>(base*(1+raise)^B13)*(1+bonus)</f>
-        <v>93399.992454999971</v>
+        <v>139185.05784715715</v>
       </c>
     </row>
     <row r="14" spans="2:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -26913,7 +28421,7 @@
       </c>
       <c r="C14" s="35">
         <f>SUM(C9:C13)</f>
-        <v>453399.48945499992</v>
+        <v>640000.14523942047</v>
       </c>
     </row>
   </sheetData>
@@ -26940,686 +28448,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A599BE6-2460-4FFE-AEBD-9B11D5253C2E}">
-  <sheetPr>
-    <outlinePr summaryBelow="0"/>
-  </sheetPr>
-  <dimension ref="B1:G18"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="11.5546875" bestFit="1" customWidth="1" outlineLevel="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-    </row>
-    <row r="3" spans="2:7" ht="15.6" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="64.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="24"/>
-      <c r="C4" s="24"/>
-      <c r="E4" s="32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-    </row>
-    <row r="6" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="24"/>
-      <c r="C6" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="18">
-        <v>100000</v>
-      </c>
-      <c r="E6" s="29">
-        <v>100000</v>
-      </c>
-      <c r="F6" s="29">
-        <v>80000</v>
-      </c>
-      <c r="G6" s="29">
-        <v>120000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="24"/>
-      <c r="C7" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="19">
-        <v>0.1</v>
-      </c>
-      <c r="E7" s="30">
-        <v>0.1</v>
-      </c>
-      <c r="F7" s="30">
-        <v>0.15</v>
-      </c>
-      <c r="G7" s="30">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="24"/>
-      <c r="C8" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="20">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="E8" s="31">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F8" s="31">
-        <v>1.2E-2</v>
-      </c>
-      <c r="G8" s="31">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-    </row>
-    <row r="10" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="24"/>
-      <c r="C10" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="18">
-        <v>110000</v>
-      </c>
-      <c r="E10" s="18">
-        <v>110000</v>
-      </c>
-      <c r="F10" s="18">
-        <v>92000</v>
-      </c>
-      <c r="G10" s="18">
-        <v>126000</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
-      <c r="C11" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="D11" s="18">
-        <v>111650</v>
-      </c>
-      <c r="E11" s="18">
-        <v>111650</v>
-      </c>
-      <c r="F11" s="18">
-        <v>93104</v>
-      </c>
-      <c r="G11" s="18">
-        <v>127008</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
-      <c r="C12" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="18">
-        <v>113324.75</v>
-      </c>
-      <c r="E12" s="18">
-        <v>113324.75</v>
-      </c>
-      <c r="F12" s="18">
-        <v>94221.248000000007</v>
-      </c>
-      <c r="G12" s="18">
-        <v>128024.064</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="18">
-        <v>115024.62125</v>
-      </c>
-      <c r="E13" s="18">
-        <v>115024.62125</v>
-      </c>
-      <c r="F13" s="18">
-        <v>95351.902975999998</v>
-      </c>
-      <c r="G13" s="18">
-        <v>129048.25651200001</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="24"/>
-      <c r="C14" s="24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="18">
-        <v>116749.99056875</v>
-      </c>
-      <c r="E14" s="18">
-        <v>116749.99056875</v>
-      </c>
-      <c r="F14" s="18">
-        <v>96496.125811712001</v>
-      </c>
-      <c r="G14" s="18">
-        <v>130080.64256409599</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="15" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="26"/>
-      <c r="C15" s="26" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="33">
-        <v>566749.36181875004</v>
-      </c>
-      <c r="E15" s="33">
-        <v>566749.36181875004</v>
-      </c>
-      <c r="F15" s="33">
-        <v>471173.27678771201</v>
-      </c>
-      <c r="G15" s="33">
-        <v>640160.96307609603</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C16C6870-2130-42B8-85C2-144B24EA12A8}">
-  <dimension ref="A1:G29"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="1" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7"/>
-      <c r="B6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7"/>
-      <c r="B7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" collapsed="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E15" s="49" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="51">
-        <v>640000.63710000005</v>
-      </c>
-      <c r="E16" s="51">
-        <v>640000.63710000005</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="49" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="49" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D21" s="52">
-        <v>0.20547045696368638</v>
-      </c>
-      <c r="E21" s="52">
-        <v>0.20547045696368638</v>
-      </c>
-      <c r="F21" s="50" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="53">
-        <v>0.03</v>
-      </c>
-      <c r="E22" s="53">
-        <v>0.03</v>
-      </c>
-      <c r="F22" s="48" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="49" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="49" t="s">
-        <v>51</v>
-      </c>
-      <c r="D26" s="49" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="49" t="s">
-        <v>58</v>
-      </c>
-      <c r="F26" s="49" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" s="49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B27" s="50" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="D27" s="54">
-        <v>640000.64</v>
-      </c>
-      <c r="E27" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="F27" s="50" t="s">
-        <v>64</v>
-      </c>
-      <c r="G27" s="50">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B28" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D28" s="52">
-        <v>0.20547045696368638</v>
-      </c>
-      <c r="E28" s="50" t="s">
-        <v>65</v>
-      </c>
-      <c r="F28" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="G28" s="50">
-        <v>4.4529543036313624E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="53">
-        <v>0.03</v>
-      </c>
-      <c r="E29" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="F29" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="G29" s="48">
-        <v>5.0000000000000044E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B251B97-0E72-44DD-A752-20F45B6DB03B}">
-  <dimension ref="A1:J14"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="2.109375" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.109375" customWidth="1"/>
-    <col min="6" max="6" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="2.109375" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="55"/>
-      <c r="C6" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="55"/>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="56" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="D8" s="51">
-        <v>640000.63710000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="55"/>
-      <c r="C11" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="55"/>
-      <c r="F11" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="I11" s="55" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="55" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="56" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="56" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="F12" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>75</v>
-      </c>
-      <c r="I12" s="56" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="56" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="50" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="52">
-        <v>0.20547045696368638</v>
-      </c>
-      <c r="F13" s="52">
-        <v>0</v>
-      </c>
-      <c r="G13" s="52">
-        <v>530913.57999999996</v>
-      </c>
-      <c r="I13" s="52">
-        <v>0.25</v>
-      </c>
-      <c r="J13" s="52">
-        <v>663641.98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="48" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="53">
-        <v>0.03</v>
-      </c>
-      <c r="F14" s="53">
-        <v>0</v>
-      </c>
-      <c r="G14" s="53">
-        <v>602735.23</v>
-      </c>
-      <c r="I14" s="53">
-        <v>0.04</v>
-      </c>
-      <c r="J14" s="53">
-        <v>646429.42000000004</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>